<commit_message>
New app Artes y oficios
</commit_message>
<xml_diff>
--- a/docs/plantillas/Plantilla_Asistencias.xlsx
+++ b/docs/plantillas/Plantilla_Asistencias.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PERSONAL\JUAN\CORPOCEMPED\ProyectoSistemas\SistemaCORPOCEMPED\public\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Estudiante\Documents\SISTEMAS\SistemaCORPOCEMPED\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F52AD6-D054-43B9-9E52-6CFF860A91CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORMATO" sheetId="1" r:id="rId1"/>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -204,15 +205,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -389,8 +388,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="47">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,43 +433,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,11 +471,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +523,13 @@
     <xdr:ext cx="1038225" cy="638175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.png" descr="https://www.medellin.gov.co/Isolucion/Medios4AlcaldiaMedellin/1f59f74f315740a3ac69be0e9813369c.png"/>
+        <xdr:cNvPr id="2" name="image1.png" descr="https://www.medellin.gov.co/Isolucion/Medios4AlcaldiaMedellin/1f59f74f315740a3ac69be0e9813369c.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -743,11 +747,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,85 +775,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="33" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="35"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:32" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="36" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="34"/>
+      <c r="N3" s="26"/>
     </row>
     <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -876,57 +880,57 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
     </row>
-    <row r="6" spans="1:32" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="17"/>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="42" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="43" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="42" t="s">
         <v>20</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="22"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="22"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="22"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="22"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -939,15 +943,15 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="45" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="6" t="s">
         <v>12</v>
       </c>
@@ -957,12 +961,12 @@
       <c r="I8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="25"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
       <c r="N8" s="8" t="s">
         <v>16</v>
       </c>
@@ -970,18 +974,18 @@
     </row>
     <row r="9" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="23"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="25"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="13"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
@@ -1004,18 +1008,18 @@
     </row>
     <row r="10" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="23"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="25"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="13"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -1038,18 +1042,18 @@
     </row>
     <row r="11" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="25"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="23"/>
+      <c r="H11" s="11"/>
       <c r="I11" s="12"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="25"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="13"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
@@ -1072,18 +1076,18 @@
     </row>
     <row r="12" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="25"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="23"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="12"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="25"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="13"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
@@ -1106,18 +1110,18 @@
     </row>
     <row r="13" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="25"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
+      <c r="F13" s="45"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="23"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="12"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="25"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="45"/>
       <c r="N13" s="13"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -1140,18 +1144,18 @@
     </row>
     <row r="14" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="25"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="23"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="25"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="45"/>
       <c r="N14" s="13"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
@@ -1174,18 +1178,18 @@
     </row>
     <row r="15" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="25"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="23"/>
+      <c r="H15" s="11"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="25"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
       <c r="N15" s="13"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -1208,18 +1212,18 @@
     </row>
     <row r="16" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="25"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="23"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="12"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="25"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="45"/>
       <c r="N16" s="13"/>
       <c r="O16" s="14"/>
       <c r="P16" s="14"/>
@@ -1242,18 +1246,18 @@
     </row>
     <row r="17" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="23"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="12"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="25"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="45"/>
       <c r="N17" s="13"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
@@ -1276,18 +1280,18 @@
     </row>
     <row r="18" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="23"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="12"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="25"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="45"/>
       <c r="N18" s="13"/>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
@@ -1310,18 +1314,18 @@
     </row>
     <row r="19" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="25"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+      <c r="F19" s="45"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="23"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="12"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="25"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="13"/>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
@@ -1344,18 +1348,18 @@
     </row>
     <row r="20" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="25"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="24"/>
-      <c r="F20" s="25"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="23"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="12"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="25"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="45"/>
       <c r="N20" s="13"/>
       <c r="O20" s="14"/>
       <c r="P20" s="14"/>
@@ -1378,18 +1382,18 @@
     </row>
     <row r="21" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="25"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="25"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="23"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="12"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="25"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="45"/>
       <c r="N21" s="13"/>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
@@ -1412,18 +1416,18 @@
     </row>
     <row r="22" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="25"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="23"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="12"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="25"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="45"/>
       <c r="N22" s="13"/>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
@@ -1446,18 +1450,18 @@
     </row>
     <row r="23" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="25"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="23"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="12"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="25"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="45"/>
       <c r="N23" s="13"/>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
@@ -1480,18 +1484,18 @@
     </row>
     <row r="24" spans="1:32" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="25"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="45"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="25"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="23"/>
+      <c r="H24" s="11"/>
       <c r="I24" s="12"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="25"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="45"/>
       <c r="N24" s="13"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
@@ -2492,13 +2496,42 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="N2:N3"/>
@@ -2515,42 +2548,13 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>

</xml_diff>